<commit_message>
09/12/2024 - preparing for new version
</commit_message>
<xml_diff>
--- a/XLSX/Сорта R. nígrum башкирской селекции.xlsx
+++ b/XLSX/Сорта R. nígrum башкирской селекции.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-15" yWindow="-15" windowWidth="28830" windowHeight="7305" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
@@ -407,7 +407,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W61"/>
+  <dimension ref="A1:W54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2392,155 +2392,155 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>8.5</v>
+        <v>7.6</v>
       </c>
       <c r="B28" t="n">
-        <v>4.6</v>
+        <v>2.8</v>
       </c>
       <c r="C28" t="n">
-        <v>1.847826086956522</v>
+        <v>2.714285714285714</v>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>9.6</v>
       </c>
       <c r="E28" t="n">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="F28" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G28" t="n">
-        <v>3.529411764705882</v>
+        <v>6.399999999999999</v>
       </c>
       <c r="H28" t="n">
-        <v>5.4</v>
+        <v>4</v>
       </c>
       <c r="I28" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J28" t="n">
-        <v>5.3</v>
+        <v>4</v>
       </c>
       <c r="K28" t="n">
-        <v>5.3</v>
+        <v>4.8</v>
       </c>
       <c r="L28" t="n">
-        <v>6</v>
+        <v>4.1</v>
       </c>
       <c r="M28" t="n">
         <v>6</v>
       </c>
       <c r="N28" t="n">
-        <v>5.2</v>
+        <v>4.8</v>
       </c>
       <c r="O28" t="n">
         <v>5</v>
       </c>
       <c r="P28" t="n">
-        <v>4.3</v>
+        <v>4.8</v>
       </c>
       <c r="Q28" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R28" t="n">
-        <v>3.1</v>
+        <v>5</v>
       </c>
       <c r="S28" t="n">
         <v>5</v>
       </c>
       <c r="T28" t="n">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="U28" t="n">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="V28" t="n">
-        <v>2</v>
+        <v>2.6</v>
       </c>
       <c r="W28" t="n">
-        <v>3</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>8.300000000000001</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="B29" t="n">
         <v>3.5</v>
       </c>
       <c r="C29" t="n">
-        <v>2.371428571428571</v>
+        <v>2.514285714285715</v>
       </c>
       <c r="D29" t="n">
-        <v>10</v>
+        <v>9.6</v>
       </c>
       <c r="E29" t="n">
         <v>1.8</v>
       </c>
       <c r="F29" t="n">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="G29" t="n">
-        <v>5.555555555555555</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="H29" t="n">
-        <v>5.4</v>
+        <v>5.5</v>
       </c>
       <c r="I29" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="J29" t="n">
+        <v>5</v>
+      </c>
+      <c r="K29" t="n">
         <v>6</v>
       </c>
-      <c r="J29" t="n">
-        <v>5.3</v>
-      </c>
-      <c r="K29" t="n">
-        <v>5.3</v>
-      </c>
       <c r="L29" t="n">
-        <v>6</v>
+        <v>5.1</v>
       </c>
       <c r="M29" t="n">
         <v>6</v>
       </c>
       <c r="N29" t="n">
-        <v>5.2</v>
+        <v>5.1</v>
       </c>
       <c r="O29" t="n">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="P29" t="n">
-        <v>4.3</v>
+        <v>4.5</v>
       </c>
       <c r="Q29" t="n">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="R29" t="n">
-        <v>3.1</v>
+        <v>2.8</v>
       </c>
       <c r="S29" t="n">
         <v>5</v>
       </c>
       <c r="T29" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U29" t="n">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="V29" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="W29" t="n">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>6.1</v>
+        <v>7.1</v>
       </c>
       <c r="B30" t="n">
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="C30" t="n">
-        <v>1.848484848484848</v>
+        <v>2.366666666666667</v>
       </c>
       <c r="D30" t="n">
         <v>8</v>
@@ -2549,7 +2549,7 @@
         <v>1.5</v>
       </c>
       <c r="F30" t="n">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="G30" t="n">
         <v>5.333333333333333</v>
@@ -2558,214 +2558,214 @@
         <v>4</v>
       </c>
       <c r="I30" t="n">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="J30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K30" t="n">
+        <v>5</v>
+      </c>
+      <c r="L30" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="M30" t="n">
         <v>6</v>
       </c>
-      <c r="L30" t="n">
-        <v>4</v>
-      </c>
-      <c r="M30" t="n">
-        <v>5.5</v>
-      </c>
       <c r="N30" t="n">
-        <v>3</v>
+        <v>4.3</v>
       </c>
       <c r="O30" t="n">
         <v>5</v>
       </c>
       <c r="P30" t="n">
-        <v>4.5</v>
+        <v>4.3</v>
       </c>
       <c r="Q30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R30" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T30" t="n">
-        <v>1.5</v>
+        <v>3.2</v>
       </c>
       <c r="U30" t="n">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="V30" t="n">
-        <v>2.8</v>
+        <v>2.5</v>
       </c>
       <c r="W30" t="n">
-        <v>4.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>6.2</v>
+        <v>7.6</v>
       </c>
       <c r="B31" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="C31" t="n">
-        <v>2.066666666666667</v>
+        <v>3.04</v>
       </c>
       <c r="D31" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>1.7</v>
+        <v>1.8</v>
       </c>
       <c r="F31" t="n">
         <v>4</v>
       </c>
       <c r="G31" t="n">
-        <v>4.705882352941177</v>
+        <v>5.555555555555555</v>
       </c>
       <c r="H31" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="I31" t="n">
-        <v>3.5</v>
+        <v>4.1</v>
       </c>
       <c r="J31" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K31" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L31" t="n">
-        <v>3</v>
+        <v>5.1</v>
       </c>
       <c r="M31" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N31" t="n">
-        <v>4</v>
+        <v>5.1</v>
       </c>
       <c r="O31" t="n">
-        <v>4</v>
+        <v>5.1</v>
       </c>
       <c r="P31" t="n">
-        <v>4</v>
+        <v>5.3</v>
       </c>
       <c r="Q31" t="n">
-        <v>4</v>
+        <v>5.3</v>
       </c>
       <c r="R31" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="S31" t="n">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="T31" t="n">
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="U31" t="n">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="V31" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W31" t="n">
-        <v>4</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>7.5</v>
+        <v>9.1</v>
       </c>
       <c r="B32" t="n">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="C32" t="n">
-        <v>2.142857142857143</v>
+        <v>2.757575757575758</v>
       </c>
       <c r="D32" t="n">
-        <v>8.199999999999999</v>
+        <v>10</v>
       </c>
       <c r="E32" t="n">
         <v>2</v>
       </c>
       <c r="F32" t="n">
-        <v>4.1</v>
+        <v>4.8</v>
       </c>
       <c r="G32" t="n">
-        <v>4.1</v>
+        <v>5</v>
       </c>
       <c r="H32" t="n">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="I32" t="n">
         <v>5</v>
       </c>
       <c r="J32" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K32" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L32" t="n">
         <v>5</v>
       </c>
       <c r="M32" t="n">
-        <v>4.9</v>
+        <v>4.5</v>
       </c>
       <c r="N32" t="n">
-        <v>4.2</v>
+        <v>6</v>
       </c>
       <c r="O32" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P32" t="n">
-        <v>2.8</v>
+        <v>5.5</v>
       </c>
       <c r="Q32" t="n">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="R32" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S32" t="n">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="T32" t="n">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="U32" t="n">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="V32" t="n">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="W32" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>7</v>
+        <v>6.5</v>
       </c>
       <c r="B33" t="n">
-        <v>3.5</v>
+        <v>2.8</v>
       </c>
       <c r="C33" t="n">
-        <v>2</v>
+        <v>2.321428571428572</v>
       </c>
       <c r="D33" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E33" t="n">
         <v>1.5</v>
       </c>
       <c r="F33" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G33" t="n">
-        <v>4</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="H33" t="n">
         <v>4</v>
@@ -2783,34 +2783,34 @@
         <v>5</v>
       </c>
       <c r="M33" t="n">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="N33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P33" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="Q33" t="n">
         <v>5</v>
       </c>
       <c r="R33" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S33" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T33" t="n">
-        <v>4.2</v>
+        <v>3</v>
       </c>
       <c r="U33" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="V33" t="n">
-        <v>4.1</v>
+        <v>2.5</v>
       </c>
       <c r="W33" t="n">
         <v>5</v>
@@ -2818,238 +2818,238 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>7.7</v>
+        <v>5.8</v>
       </c>
       <c r="B34" t="n">
+        <v>3</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1.933333333333333</v>
+      </c>
+      <c r="D34" t="n">
+        <v>6</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F34" t="n">
+        <v>3</v>
+      </c>
+      <c r="G34" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="H34" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="I34" t="n">
+        <v>4</v>
+      </c>
+      <c r="J34" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K34" t="n">
+        <v>4</v>
+      </c>
+      <c r="L34" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="M34" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N34" t="n">
         <v>3.8</v>
       </c>
-      <c r="C34" t="n">
-        <v>2.026315789473685</v>
-      </c>
-      <c r="D34" t="n">
-        <v>8</v>
-      </c>
-      <c r="E34" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="F34" t="n">
-        <v>4</v>
-      </c>
-      <c r="G34" t="n">
-        <v>4.444444444444445</v>
-      </c>
-      <c r="H34" t="n">
-        <v>5</v>
-      </c>
-      <c r="I34" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="J34" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="K34" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="L34" t="n">
-        <v>5</v>
-      </c>
-      <c r="M34" t="n">
-        <v>5</v>
-      </c>
-      <c r="N34" t="n">
-        <v>4.5</v>
-      </c>
       <c r="O34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P34" t="n">
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="Q34" t="n">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="R34" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S34" t="n">
         <v>4.5</v>
       </c>
       <c r="T34" t="n">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="U34" t="n">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="V34" t="n">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="W34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>7.6</v>
+        <v>5.8</v>
       </c>
       <c r="B35" t="n">
-        <v>2.8</v>
+        <v>2.5</v>
       </c>
       <c r="C35" t="n">
-        <v>2.714285714285714</v>
+        <v>2.32</v>
       </c>
       <c r="D35" t="n">
-        <v>9.6</v>
+        <v>8</v>
       </c>
       <c r="E35" t="n">
         <v>1.5</v>
       </c>
       <c r="F35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G35" t="n">
-        <v>6.399999999999999</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="H35" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="I35" t="n">
         <v>4</v>
       </c>
       <c r="J35" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="K35" t="n">
-        <v>4.8</v>
+        <v>4</v>
       </c>
       <c r="L35" t="n">
-        <v>4.1</v>
+        <v>2.1</v>
       </c>
       <c r="M35" t="n">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="N35" t="n">
-        <v>4.8</v>
+        <v>3.8</v>
       </c>
       <c r="O35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P35" t="n">
-        <v>4.8</v>
+        <v>4.2</v>
       </c>
       <c r="Q35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S35" t="n">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="T35" t="n">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="U35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V35" t="n">
-        <v>2.6</v>
+        <v>1.2</v>
       </c>
       <c r="W35" t="n">
-        <v>4.8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>8.800000000000001</v>
+        <v>7</v>
       </c>
       <c r="B36" t="n">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="C36" t="n">
-        <v>2.514285714285715</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="D36" t="n">
-        <v>9.6</v>
+        <v>10</v>
       </c>
       <c r="E36" t="n">
-        <v>1.8</v>
+        <v>1.2</v>
       </c>
       <c r="F36" t="n">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="G36" t="n">
-        <v>5.333333333333333</v>
+        <v>8.333333333333334</v>
       </c>
       <c r="H36" t="n">
+        <v>4</v>
+      </c>
+      <c r="I36" t="n">
+        <v>4</v>
+      </c>
+      <c r="J36" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="K36" t="n">
+        <v>5</v>
+      </c>
+      <c r="L36" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="M36" t="n">
+        <v>5</v>
+      </c>
+      <c r="N36" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="O36" t="n">
+        <v>6</v>
+      </c>
+      <c r="P36" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>5</v>
+      </c>
+      <c r="R36" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="S36" t="n">
+        <v>5</v>
+      </c>
+      <c r="T36" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="U36" t="n">
         <v>5.5</v>
       </c>
-      <c r="I36" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="J36" t="n">
-        <v>5</v>
-      </c>
-      <c r="K36" t="n">
-        <v>6</v>
-      </c>
-      <c r="L36" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="M36" t="n">
-        <v>6</v>
-      </c>
-      <c r="N36" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="O36" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="P36" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="Q36" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="R36" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="S36" t="n">
-        <v>5</v>
-      </c>
-      <c r="T36" t="n">
-        <v>4</v>
-      </c>
-      <c r="U36" t="n">
-        <v>5</v>
-      </c>
       <c r="V36" t="n">
         <v>2.5</v>
       </c>
       <c r="W36" t="n">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>7.1</v>
+        <v>7</v>
       </c>
       <c r="B37" t="n">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="C37" t="n">
-        <v>2.366666666666667</v>
+        <v>2</v>
       </c>
       <c r="D37" t="n">
         <v>8</v>
       </c>
       <c r="E37" t="n">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="F37" t="n">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="G37" t="n">
-        <v>5.333333333333333</v>
+        <v>5</v>
       </c>
       <c r="H37" t="n">
         <v>4</v>
@@ -3061,182 +3061,182 @@
         <v>4</v>
       </c>
       <c r="K37" t="n">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="L37" t="n">
+        <v>4</v>
+      </c>
+      <c r="M37" t="n">
+        <v>5</v>
+      </c>
+      <c r="N37" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="O37" t="n">
+        <v>5</v>
+      </c>
+      <c r="P37" t="n">
         <v>4.1</v>
       </c>
-      <c r="M37" t="n">
-        <v>6</v>
-      </c>
-      <c r="N37" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="O37" t="n">
-        <v>5</v>
-      </c>
-      <c r="P37" t="n">
-        <v>4.3</v>
-      </c>
       <c r="Q37" t="n">
         <v>5</v>
       </c>
       <c r="R37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S37" t="n">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="T37" t="n">
-        <v>3.2</v>
+        <v>2.1</v>
       </c>
       <c r="U37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V37" t="n">
         <v>2.5</v>
       </c>
       <c r="W37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>7.6</v>
+        <v>5.5</v>
       </c>
       <c r="B38" t="n">
-        <v>2.5</v>
+        <v>3.2</v>
       </c>
       <c r="C38" t="n">
-        <v>3.04</v>
+        <v>1.71875</v>
       </c>
       <c r="D38" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E38" t="n">
-        <v>1.8</v>
+        <v>1.2</v>
       </c>
       <c r="F38" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="G38" t="n">
-        <v>5.555555555555555</v>
+        <v>5.833333333333334</v>
       </c>
       <c r="H38" t="n">
-        <v>4</v>
+        <v>3.2</v>
       </c>
       <c r="I38" t="n">
-        <v>4.1</v>
+        <v>4.5</v>
       </c>
       <c r="J38" t="n">
-        <v>5</v>
+        <v>3.2</v>
       </c>
       <c r="K38" t="n">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="L38" t="n">
-        <v>5.1</v>
+        <v>3.5</v>
       </c>
       <c r="M38" t="n">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="N38" t="n">
-        <v>5.1</v>
+        <v>4.5</v>
       </c>
       <c r="O38" t="n">
-        <v>5.1</v>
+        <v>4.5</v>
       </c>
       <c r="P38" t="n">
-        <v>5.3</v>
+        <v>3.8</v>
       </c>
       <c r="Q38" t="n">
-        <v>5.3</v>
+        <v>4.5</v>
       </c>
       <c r="R38" t="n">
         <v>4</v>
       </c>
       <c r="S38" t="n">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="T38" t="n">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="U38" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="V38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W38" t="n">
-        <v>4.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>9.1</v>
+        <v>6.1</v>
       </c>
       <c r="B39" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="C39" t="n">
-        <v>2.757575757575758</v>
+        <v>1.90625</v>
       </c>
       <c r="D39" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F39" t="n">
-        <v>4.8</v>
+        <v>4</v>
       </c>
       <c r="G39" t="n">
-        <v>5</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="H39" t="n">
-        <v>5</v>
+        <v>3.2</v>
       </c>
       <c r="I39" t="n">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="J39" t="n">
-        <v>5</v>
+        <v>3.2</v>
       </c>
       <c r="K39" t="n">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="L39" t="n">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="M39" t="n">
         <v>4.5</v>
       </c>
       <c r="N39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O39" t="n">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="P39" t="n">
-        <v>5.5</v>
+        <v>3.8</v>
       </c>
       <c r="Q39" t="n">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
       <c r="R39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S39" t="n">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="T39" t="n">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="U39" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="V39" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="W39" t="n">
         <v>3</v>
@@ -3244,46 +3244,46 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>6.5</v>
+        <v>6.2</v>
       </c>
       <c r="B40" t="n">
-        <v>2.8</v>
+        <v>3.6</v>
       </c>
       <c r="C40" t="n">
-        <v>2.321428571428572</v>
+        <v>1.722222222222222</v>
       </c>
       <c r="D40" t="n">
         <v>8</v>
       </c>
       <c r="E40" t="n">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="F40" t="n">
         <v>4</v>
       </c>
       <c r="G40" t="n">
-        <v>5.333333333333333</v>
+        <v>5</v>
       </c>
       <c r="H40" t="n">
         <v>4</v>
       </c>
       <c r="I40" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K40" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M40" t="n">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="N40" t="n">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="O40" t="n">
         <v>5</v>
@@ -3295,90 +3295,90 @@
         <v>5</v>
       </c>
       <c r="R40" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S40" t="n">
         <v>5</v>
       </c>
       <c r="T40" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U40" t="n">
-        <v>4.5</v>
+        <v>2</v>
       </c>
       <c r="V40" t="n">
-        <v>2.5</v>
+        <v>1.2</v>
       </c>
       <c r="W40" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>5.8</v>
+        <v>5.9</v>
       </c>
       <c r="B41" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C41" t="n">
-        <v>1.933333333333333</v>
+        <v>1.475</v>
       </c>
       <c r="D41" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E41" t="n">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="F41" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G41" t="n">
-        <v>7.5</v>
+        <v>8.333333333333334</v>
       </c>
       <c r="H41" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="I41" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J41" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="K41" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L41" t="n">
-        <v>2.1</v>
+        <v>4</v>
       </c>
       <c r="M41" t="n">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="N41" t="n">
-        <v>3.8</v>
+        <v>4.5</v>
       </c>
       <c r="O41" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P41" t="n">
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="Q41" t="n">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="R41" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S41" t="n">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="T41" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U41" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V41" t="n">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="W41" t="n">
         <v>2</v>
@@ -3386,13 +3386,13 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>5.8</v>
+        <v>6.7</v>
       </c>
       <c r="B42" t="n">
-        <v>2.5</v>
+        <v>3.2</v>
       </c>
       <c r="C42" t="n">
-        <v>2.32</v>
+        <v>2.09375</v>
       </c>
       <c r="D42" t="n">
         <v>8</v>
@@ -3407,75 +3407,75 @@
         <v>5.333333333333333</v>
       </c>
       <c r="H42" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="I42" t="n">
         <v>4</v>
       </c>
       <c r="J42" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="K42" t="n">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="L42" t="n">
-        <v>2.1</v>
+        <v>4.1</v>
       </c>
       <c r="M42" t="n">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="N42" t="n">
-        <v>3.8</v>
+        <v>4.2</v>
       </c>
       <c r="O42" t="n">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="P42" t="n">
-        <v>4.2</v>
+        <v>5</v>
       </c>
       <c r="Q42" t="n">
         <v>5</v>
       </c>
       <c r="R42" t="n">
-        <v>4</v>
+        <v>4.1</v>
       </c>
       <c r="S42" t="n">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="T42" t="n">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="U42" t="n">
-        <v>4</v>
+        <v>4.1</v>
       </c>
       <c r="V42" t="n">
-        <v>1.2</v>
+        <v>2.5</v>
       </c>
       <c r="W42" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="B43" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="C43" t="n">
+        <v>2.275862068965517</v>
+      </c>
+      <c r="D43" t="n">
         <v>7</v>
       </c>
-      <c r="B43" t="n">
-        <v>3</v>
-      </c>
-      <c r="C43" t="n">
-        <v>2.333333333333333</v>
-      </c>
-      <c r="D43" t="n">
-        <v>10</v>
-      </c>
       <c r="E43" t="n">
-        <v>1.2</v>
+        <v>1.7</v>
       </c>
       <c r="F43" t="n">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="G43" t="n">
-        <v>8.333333333333334</v>
+        <v>4.11764705882353</v>
       </c>
       <c r="H43" t="n">
         <v>4</v>
@@ -3484,114 +3484,114 @@
         <v>4</v>
       </c>
       <c r="J43" t="n">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="K43" t="n">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="L43" t="n">
-        <v>4.3</v>
+        <v>4</v>
       </c>
       <c r="M43" t="n">
         <v>5</v>
       </c>
       <c r="N43" t="n">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="O43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P43" t="n">
-        <v>5</v>
+        <v>4.1</v>
       </c>
       <c r="Q43" t="n">
         <v>5</v>
       </c>
       <c r="R43" t="n">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="S43" t="n">
         <v>5</v>
       </c>
       <c r="T43" t="n">
-        <v>3.5</v>
+        <v>2.1</v>
       </c>
       <c r="U43" t="n">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="V43" t="n">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="W43" t="n">
-        <v>4.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B44" t="n">
         <v>3.5</v>
       </c>
       <c r="C44" t="n">
-        <v>2</v>
+        <v>2.285714285714286</v>
       </c>
       <c r="D44" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E44" t="n">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
       <c r="F44" t="n">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="G44" t="n">
         <v>5</v>
       </c>
       <c r="H44" t="n">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="I44" t="n">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="J44" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K44" t="n">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="L44" t="n">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="M44" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N44" t="n">
-        <v>4.5</v>
+        <v>4.8</v>
       </c>
       <c r="O44" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P44" t="n">
-        <v>4.1</v>
+        <v>3.8</v>
       </c>
       <c r="Q44" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S44" t="n">
         <v>5.5</v>
       </c>
       <c r="T44" t="n">
-        <v>2.1</v>
+        <v>3</v>
       </c>
       <c r="U44" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="V44" t="n">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="W44" t="n">
         <v>3</v>
@@ -3599,1208 +3599,711 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="B45" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="C45" t="n">
+        <v>2.421052631578947</v>
+      </c>
+      <c r="D45" t="n">
+        <v>10</v>
+      </c>
+      <c r="E45" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F45" t="n">
+        <v>5</v>
+      </c>
+      <c r="G45" t="n">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="H45" t="n">
+        <v>5</v>
+      </c>
+      <c r="I45" t="n">
         <v>5.5</v>
       </c>
-      <c r="B45" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="C45" t="n">
-        <v>1.71875</v>
-      </c>
-      <c r="D45" t="n">
-        <v>7</v>
-      </c>
-      <c r="E45" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="F45" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="G45" t="n">
-        <v>5.833333333333334</v>
-      </c>
-      <c r="H45" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="I45" t="n">
-        <v>4.5</v>
-      </c>
       <c r="J45" t="n">
-        <v>3.2</v>
+        <v>5</v>
       </c>
       <c r="K45" t="n">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="L45" t="n">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="M45" t="n">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="N45" t="n">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="O45" t="n">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="P45" t="n">
-        <v>3.8</v>
+        <v>4.3</v>
       </c>
       <c r="Q45" t="n">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="R45" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S45" t="n">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="T45" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="U45" t="n">
         <v>4</v>
       </c>
       <c r="V45" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="W45" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>6.1</v>
+        <v>6.6</v>
       </c>
       <c r="B46" t="n">
-        <v>3.2</v>
+        <v>2.9</v>
       </c>
       <c r="C46" t="n">
-        <v>1.90625</v>
+        <v>2.275862068965517</v>
       </c>
       <c r="D46" t="n">
         <v>8</v>
       </c>
       <c r="E46" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="F46" t="n">
+        <v>4</v>
+      </c>
+      <c r="G46" t="n">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="H46" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="I46" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J46" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="K46" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="L46" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="M46" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="N46" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="O46" t="n">
+        <v>4</v>
+      </c>
+      <c r="P46" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>3</v>
+      </c>
+      <c r="R46" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="S46" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="T46" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="U46" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="V46" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="W46" t="n">
         <v>1.5</v>
-      </c>
-      <c r="F46" t="n">
-        <v>4</v>
-      </c>
-      <c r="G46" t="n">
-        <v>5.333333333333333</v>
-      </c>
-      <c r="H46" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="I46" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="J46" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="K46" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="L46" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="M46" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="N46" t="n">
-        <v>5</v>
-      </c>
-      <c r="O46" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="P46" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="Q46" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="R46" t="n">
-        <v>4</v>
-      </c>
-      <c r="S46" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="T46" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="U46" t="n">
-        <v>4</v>
-      </c>
-      <c r="V46" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="W46" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>6.2</v>
+        <v>6.4</v>
       </c>
       <c r="B47" t="n">
-        <v>3.6</v>
+        <v>2.6</v>
       </c>
       <c r="C47" t="n">
-        <v>1.722222222222222</v>
+        <v>2.461538461538462</v>
       </c>
       <c r="D47" t="n">
         <v>8</v>
       </c>
       <c r="E47" t="n">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
       <c r="F47" t="n">
         <v>4</v>
       </c>
       <c r="G47" t="n">
-        <v>5</v>
+        <v>4.444444444444445</v>
       </c>
       <c r="H47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I47" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J47" t="n">
-        <v>4</v>
+        <v>4.4</v>
       </c>
       <c r="K47" t="n">
-        <v>6</v>
+        <v>3.8</v>
       </c>
       <c r="L47" t="n">
-        <v>4</v>
+        <v>5.3</v>
       </c>
       <c r="M47" t="n">
-        <v>5</v>
+        <v>3.8</v>
       </c>
       <c r="N47" t="n">
-        <v>4.5</v>
+        <v>2</v>
       </c>
       <c r="O47" t="n">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="P47" t="n">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="Q47" t="n">
-        <v>5</v>
+        <v>4.3</v>
       </c>
       <c r="R47" t="n">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="S47" t="n">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="T47" t="n">
         <v>4</v>
       </c>
       <c r="U47" t="n">
-        <v>2</v>
+        <v>3.8</v>
       </c>
       <c r="V47" t="n">
-        <v>1.2</v>
+        <v>3</v>
       </c>
       <c r="W47" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>5.9</v>
+        <v>6.9</v>
       </c>
       <c r="B48" t="n">
-        <v>4</v>
+        <v>2.7</v>
       </c>
       <c r="C48" t="n">
-        <v>1.475</v>
+        <v>2.555555555555555</v>
       </c>
       <c r="D48" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E48" t="n">
-        <v>1.2</v>
+        <v>1.8</v>
       </c>
       <c r="F48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G48" t="n">
-        <v>8.333333333333334</v>
+        <v>4.444444444444445</v>
       </c>
       <c r="H48" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="I48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J48" t="n">
-        <v>4</v>
+        <v>3.2</v>
       </c>
       <c r="K48" t="n">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="L48" t="n">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="M48" t="n">
-        <v>5</v>
+        <v>3.2</v>
       </c>
       <c r="N48" t="n">
-        <v>4.5</v>
+        <v>3.8</v>
       </c>
       <c r="O48" t="n">
-        <v>5</v>
+        <v>4.2</v>
       </c>
       <c r="P48" t="n">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="Q48" t="n">
-        <v>4.5</v>
+        <v>4.3</v>
       </c>
       <c r="R48" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="S48" t="n">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="T48" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U48" t="n">
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="V48" t="n">
         <v>1.5</v>
       </c>
       <c r="W48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>6.7</v>
+        <v>5.9</v>
       </c>
       <c r="B49" t="n">
-        <v>3.2</v>
+        <v>2.5</v>
       </c>
       <c r="C49" t="n">
-        <v>2.09375</v>
+        <v>2.36</v>
       </c>
       <c r="D49" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E49" t="n">
         <v>1.5</v>
       </c>
       <c r="F49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G49" t="n">
-        <v>5.333333333333333</v>
+        <v>4</v>
       </c>
       <c r="H49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K49" t="n">
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="L49" t="n">
-        <v>4.1</v>
+        <v>3.3</v>
       </c>
       <c r="M49" t="n">
-        <v>5</v>
+        <v>3.2</v>
       </c>
       <c r="N49" t="n">
-        <v>4.2</v>
+        <v>4</v>
       </c>
       <c r="O49" t="n">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="P49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q49" t="n">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="R49" t="n">
-        <v>4.1</v>
+        <v>4.4</v>
       </c>
       <c r="S49" t="n">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="T49" t="n">
-        <v>3.1</v>
+        <v>2</v>
       </c>
       <c r="U49" t="n">
-        <v>4.1</v>
+        <v>2.5</v>
       </c>
       <c r="V49" t="n">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="W49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>6.6</v>
+        <v>6.8</v>
       </c>
       <c r="B50" t="n">
-        <v>2.9</v>
+        <v>3.5</v>
       </c>
       <c r="C50" t="n">
-        <v>2.275862068965517</v>
+        <v>1.942857142857143</v>
       </c>
       <c r="D50" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E50" t="n">
-        <v>1.7</v>
+        <v>1.2</v>
       </c>
       <c r="F50" t="n">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="G50" t="n">
-        <v>4.11764705882353</v>
+        <v>5</v>
       </c>
       <c r="H50" t="n">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="I50" t="n">
         <v>4</v>
       </c>
       <c r="J50" t="n">
-        <v>4</v>
+        <v>4.1</v>
       </c>
       <c r="K50" t="n">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="L50" t="n">
-        <v>4</v>
+        <v>5.1</v>
       </c>
       <c r="M50" t="n">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="N50" t="n">
-        <v>4.2</v>
+        <v>4.1</v>
       </c>
       <c r="O50" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P50" t="n">
-        <v>4.1</v>
+        <v>4</v>
       </c>
       <c r="Q50" t="n">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="R50" t="n">
         <v>4</v>
       </c>
       <c r="S50" t="n">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="T50" t="n">
-        <v>2.1</v>
+        <v>3</v>
       </c>
       <c r="U50" t="n">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="V50" t="n">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="W50" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>8</v>
+        <v>7.2</v>
       </c>
       <c r="B51" t="n">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="C51" t="n">
-        <v>2.285714285714286</v>
+        <v>2</v>
       </c>
       <c r="D51" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E51" t="n">
-        <v>1.8</v>
+        <v>1.6</v>
       </c>
       <c r="F51" t="n">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="G51" t="n">
-        <v>5</v>
+        <v>4.375</v>
       </c>
       <c r="H51" t="n">
-        <v>5.5</v>
+        <v>3.2</v>
       </c>
       <c r="I51" t="n">
-        <v>5.5</v>
+        <v>3.2</v>
       </c>
       <c r="J51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K51" t="n">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="L51" t="n">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="M51" t="n">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="N51" t="n">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="O51" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P51" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q51" t="n">
         <v>3.8</v>
       </c>
-      <c r="Q51" t="n">
-        <v>6</v>
-      </c>
       <c r="R51" t="n">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="S51" t="n">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="T51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U51" t="n">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="V51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>9.199999999999999</v>
+        <v>8</v>
       </c>
       <c r="B52" t="n">
         <v>3.8</v>
       </c>
       <c r="C52" t="n">
-        <v>2.421052631578947</v>
+        <v>2.105263157894737</v>
       </c>
       <c r="D52" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E52" t="n">
+        <v>2</v>
+      </c>
+      <c r="F52" t="n">
+        <v>4</v>
+      </c>
+      <c r="G52" t="n">
+        <v>4</v>
+      </c>
+      <c r="H52" t="n">
+        <v>4</v>
+      </c>
+      <c r="I52" t="n">
+        <v>4</v>
+      </c>
+      <c r="J52" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="K52" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L52" t="n">
+        <v>5</v>
+      </c>
+      <c r="M52" t="n">
+        <v>5</v>
+      </c>
+      <c r="N52" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="O52" t="n">
+        <v>4</v>
+      </c>
+      <c r="P52" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="R52" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="S52" t="n">
+        <v>4</v>
+      </c>
+      <c r="T52" t="n">
+        <v>2</v>
+      </c>
+      <c r="U52" t="n">
+        <v>4</v>
+      </c>
+      <c r="V52" t="n">
+        <v>1</v>
+      </c>
+      <c r="W52" t="n">
         <v>1.5</v>
-      </c>
-      <c r="F52" t="n">
-        <v>5</v>
-      </c>
-      <c r="G52" t="n">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="H52" t="n">
-        <v>5</v>
-      </c>
-      <c r="I52" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="J52" t="n">
-        <v>5</v>
-      </c>
-      <c r="K52" t="n">
-        <v>5</v>
-      </c>
-      <c r="L52" t="n">
-        <v>6</v>
-      </c>
-      <c r="M52" t="n">
-        <v>6</v>
-      </c>
-      <c r="N52" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="O52" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="P52" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="Q52" t="n">
-        <v>5</v>
-      </c>
-      <c r="R52" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="S52" t="n">
-        <v>5</v>
-      </c>
-      <c r="T52" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="U52" t="n">
-        <v>4</v>
-      </c>
-      <c r="V52" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="W52" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>6.6</v>
+        <v>7.1</v>
       </c>
       <c r="B53" t="n">
-        <v>2.9</v>
+        <v>3.5</v>
       </c>
       <c r="C53" t="n">
-        <v>2.275862068965517</v>
+        <v>2.028571428571428</v>
       </c>
       <c r="D53" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E53" t="n">
         <v>1.2</v>
       </c>
       <c r="F53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G53" t="n">
-        <v>6.666666666666667</v>
+        <v>5</v>
       </c>
       <c r="H53" t="n">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="I53" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="J53" t="n">
-        <v>4.3</v>
+        <v>4</v>
       </c>
       <c r="K53" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="L53" t="n">
         <v>4.2</v>
       </c>
       <c r="M53" t="n">
-        <v>4.1</v>
+        <v>4</v>
       </c>
       <c r="N53" t="n">
+        <v>5</v>
+      </c>
+      <c r="O53" t="n">
+        <v>4</v>
+      </c>
+      <c r="P53" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="Q53" t="n">
+        <v>4</v>
+      </c>
+      <c r="R53" t="n">
+        <v>4</v>
+      </c>
+      <c r="S53" t="n">
         <v>3.8</v>
       </c>
-      <c r="O53" t="n">
-        <v>4</v>
-      </c>
-      <c r="P53" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q53" t="n">
-        <v>3</v>
-      </c>
-      <c r="R53" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="S53" t="n">
-        <v>3.5</v>
-      </c>
       <c r="T53" t="n">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="U53" t="n">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="V53" t="n">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="W53" t="n">
-        <v>1.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>6.4</v>
+        <v>7.4</v>
       </c>
       <c r="B54" t="n">
-        <v>2.6</v>
+        <v>3.6</v>
       </c>
       <c r="C54" t="n">
-        <v>2.461538461538462</v>
+        <v>2.055555555555556</v>
       </c>
       <c r="D54" t="n">
         <v>8</v>
       </c>
       <c r="E54" t="n">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
         <v>4</v>
       </c>
       <c r="G54" t="n">
-        <v>4.444444444444445</v>
+        <v>4</v>
       </c>
       <c r="H54" t="n">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="I54" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J54" t="n">
-        <v>4.4</v>
+        <v>5</v>
       </c>
       <c r="K54" t="n">
-        <v>3.8</v>
+        <v>4.5</v>
       </c>
       <c r="L54" t="n">
-        <v>5.3</v>
+        <v>5.2</v>
       </c>
       <c r="M54" t="n">
-        <v>3.8</v>
+        <v>5</v>
       </c>
       <c r="N54" t="n">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="O54" t="n">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="P54" t="n">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="Q54" t="n">
-        <v>4.3</v>
+        <v>4</v>
       </c>
       <c r="R54" t="n">
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
       <c r="S54" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="T54" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U54" t="n">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="V54" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W54" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>6.9</v>
-      </c>
-      <c r="B55" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="C55" t="n">
-        <v>2.555555555555555</v>
-      </c>
-      <c r="D55" t="n">
-        <v>8</v>
-      </c>
-      <c r="E55" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="F55" t="n">
-        <v>4</v>
-      </c>
-      <c r="G55" t="n">
-        <v>4.444444444444445</v>
-      </c>
-      <c r="H55" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="I55" t="n">
-        <v>4</v>
-      </c>
-      <c r="J55" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="K55" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="L55" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="M55" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="N55" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="O55" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="P55" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="Q55" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="R55" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="S55" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="T55" t="n">
-        <v>2</v>
-      </c>
-      <c r="U55" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="V55" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="W55" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="B56" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="C56" t="n">
-        <v>2.36</v>
-      </c>
-      <c r="D56" t="n">
-        <v>6</v>
-      </c>
-      <c r="E56" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="F56" t="n">
-        <v>3</v>
-      </c>
-      <c r="G56" t="n">
-        <v>4</v>
-      </c>
-      <c r="H56" t="n">
-        <v>3</v>
-      </c>
-      <c r="I56" t="n">
-        <v>3</v>
-      </c>
-      <c r="J56" t="n">
-        <v>3</v>
-      </c>
-      <c r="K56" t="n">
-        <v>3</v>
-      </c>
-      <c r="L56" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="M56" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="N56" t="n">
-        <v>4</v>
-      </c>
-      <c r="O56" t="n">
-        <v>4</v>
-      </c>
-      <c r="P56" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q56" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="R56" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="S56" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="T56" t="n">
-        <v>2</v>
-      </c>
-      <c r="U56" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="V56" t="n">
-        <v>3</v>
-      </c>
-      <c r="W56" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>6.8</v>
-      </c>
-      <c r="B57" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="C57" t="n">
-        <v>1.942857142857143</v>
-      </c>
-      <c r="D57" t="n">
-        <v>6</v>
-      </c>
-      <c r="E57" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="F57" t="n">
-        <v>3</v>
-      </c>
-      <c r="G57" t="n">
-        <v>5</v>
-      </c>
-      <c r="H57" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="I57" t="n">
-        <v>4</v>
-      </c>
-      <c r="J57" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="K57" t="n">
-        <v>4</v>
-      </c>
-      <c r="L57" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="M57" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="N57" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="O57" t="n">
-        <v>3</v>
-      </c>
-      <c r="P57" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q57" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="R57" t="n">
-        <v>4</v>
-      </c>
-      <c r="S57" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="T57" t="n">
-        <v>3</v>
-      </c>
-      <c r="U57" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="V57" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="W57" t="n">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="B58" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="C58" t="n">
-        <v>2</v>
-      </c>
-      <c r="D58" t="n">
-        <v>7</v>
-      </c>
-      <c r="E58" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="F58" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="G58" t="n">
-        <v>4.375</v>
-      </c>
-      <c r="H58" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="I58" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="J58" t="n">
-        <v>5</v>
-      </c>
-      <c r="K58" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="L58" t="n">
-        <v>5</v>
-      </c>
-      <c r="M58" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="N58" t="n">
-        <v>5</v>
-      </c>
-      <c r="O58" t="n">
-        <v>4</v>
-      </c>
-      <c r="P58" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q58" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="R58" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="S58" t="n">
-        <v>3</v>
-      </c>
-      <c r="T58" t="n">
-        <v>2</v>
-      </c>
-      <c r="U58" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="V58" t="n">
-        <v>1</v>
-      </c>
-      <c r="W58" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>8</v>
-      </c>
-      <c r="B59" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="C59" t="n">
-        <v>2.105263157894737</v>
-      </c>
-      <c r="D59" t="n">
-        <v>8</v>
-      </c>
-      <c r="E59" t="n">
-        <v>2</v>
-      </c>
-      <c r="F59" t="n">
-        <v>4</v>
-      </c>
-      <c r="G59" t="n">
-        <v>4</v>
-      </c>
-      <c r="H59" t="n">
-        <v>4</v>
-      </c>
-      <c r="I59" t="n">
-        <v>4</v>
-      </c>
-      <c r="J59" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="K59" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="L59" t="n">
-        <v>5</v>
-      </c>
-      <c r="M59" t="n">
-        <v>5</v>
-      </c>
-      <c r="N59" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="O59" t="n">
-        <v>4</v>
-      </c>
-      <c r="P59" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q59" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="R59" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="S59" t="n">
-        <v>4</v>
-      </c>
-      <c r="T59" t="n">
-        <v>2</v>
-      </c>
-      <c r="U59" t="n">
-        <v>4</v>
-      </c>
-      <c r="V59" t="n">
-        <v>1</v>
-      </c>
-      <c r="W59" t="n">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>7.1</v>
-      </c>
-      <c r="B60" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="C60" t="n">
-        <v>2.028571428571428</v>
-      </c>
-      <c r="D60" t="n">
-        <v>6</v>
-      </c>
-      <c r="E60" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="F60" t="n">
-        <v>3</v>
-      </c>
-      <c r="G60" t="n">
-        <v>5</v>
-      </c>
-      <c r="H60" t="n">
-        <v>4</v>
-      </c>
-      <c r="I60" t="n">
-        <v>4</v>
-      </c>
-      <c r="J60" t="n">
-        <v>4</v>
-      </c>
-      <c r="K60" t="n">
-        <v>4</v>
-      </c>
-      <c r="L60" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="M60" t="n">
-        <v>4</v>
-      </c>
-      <c r="N60" t="n">
-        <v>5</v>
-      </c>
-      <c r="O60" t="n">
-        <v>4</v>
-      </c>
-      <c r="P60" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="Q60" t="n">
-        <v>4</v>
-      </c>
-      <c r="R60" t="n">
-        <v>4</v>
-      </c>
-      <c r="S60" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="T60" t="n">
-        <v>2</v>
-      </c>
-      <c r="U60" t="n">
-        <v>3</v>
-      </c>
-      <c r="V60" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="W60" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>7.4</v>
-      </c>
-      <c r="B61" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="C61" t="n">
-        <v>2.055555555555556</v>
-      </c>
-      <c r="D61" t="n">
-        <v>8</v>
-      </c>
-      <c r="E61" t="n">
-        <v>2</v>
-      </c>
-      <c r="F61" t="n">
-        <v>4</v>
-      </c>
-      <c r="G61" t="n">
-        <v>4</v>
-      </c>
-      <c r="H61" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="I61" t="n">
-        <v>4</v>
-      </c>
-      <c r="J61" t="n">
-        <v>5</v>
-      </c>
-      <c r="K61" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="L61" t="n">
-        <v>5.2</v>
-      </c>
-      <c r="M61" t="n">
-        <v>5</v>
-      </c>
-      <c r="N61" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="O61" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="P61" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q61" t="n">
-        <v>4</v>
-      </c>
-      <c r="R61" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="S61" t="n">
-        <v>4</v>
-      </c>
-      <c r="T61" t="n">
-        <v>2</v>
-      </c>
-      <c r="U61" t="n">
-        <v>4</v>
-      </c>
-      <c r="V61" t="n">
-        <v>1</v>
-      </c>
-      <c r="W61" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>